<commit_message>
Updated the VO Excel Workbook
One alteration was missing.
</commit_message>
<xml_diff>
--- a/Documents/Binora_VoiceOver.xlsx
+++ b/Documents/Binora_VoiceOver.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattv\Documents\Projects\Binora\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattv\Documents\Projects\Binora\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D0B5C7-8EE1-47E3-AD46-F9BC43E26905}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA79D56-8A50-4CF2-96E8-F27822201AC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{6470154B-4374-4A9D-8537-076BDE5E7497}"/>
+    <workbookView xWindow="4905" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{6470154B-4374-4A9D-8537-076BDE5E7497}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>FileName</t>
   </si>
@@ -94,12 +94,6 @@
   </si>
   <si>
     <t>Thanks for playing We are now redirecting you to the Level Selection Menu.</t>
-  </si>
-  <si>
-    <t>QUIT</t>
-  </si>
-  <si>
-    <t>VO_QUIT</t>
   </si>
   <si>
     <t>Goodbye!</t>
@@ -140,13 +134,6 @@
     <t>VO_LS01
 …
 VO_LS05</t>
-  </si>
-  <si>
-    <t>What level would you like to play? 
-Press the Top Face Button for Pacific Beach.
-Press the Right Face Button for Cabin in the Woods.
-Press the Bottom Face Button for Haunted House.
-Press the Start Button to Quit.</t>
   </si>
   <si>
     <t>InputAction Gamepad Left Trigger Button
@@ -358,6 +345,40 @@
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>VO_MM03</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What level would you like to play? 
+Press the Top Face Button for Pacific Beach.
+Press the Right Face Button for Cabin in the Woods.
+Press the Bottom Face Button for Haunted House.
+Press the the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Special Left Button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to Quit.</t>
     </r>
   </si>
 </sst>
@@ -450,7 +471,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -597,11 +618,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -631,59 +683,71 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -999,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB574BAC-2812-4F11-90CE-F822581A55C7}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,14 +1079,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="11"/>
+      <c r="A1" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -1030,355 +1094,345 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="21"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="28"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="15" t="s">
+      <c r="G8" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="C9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="27"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" ht="189" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="27"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="23" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="27"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27"/>
-    </row>
-    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-    </row>
-    <row r="11" spans="1:7" ht="189" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="23" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="27"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
-    </row>
-    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-    </row>
-    <row r="14" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="17" t="s">
+    <row r="22" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="15" t="s">
+      <c r="D22" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="F22" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
-    </row>
-    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="23" t="s">
+    <row r="23" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="28"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="27"/>
-    </row>
-    <row r="19" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="27"/>
-    </row>
-    <row r="20" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="23" t="s">
+    <row r="24" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="23" t="s">
+    <row r="25" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="28"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-    </row>
-    <row r="26" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="27"/>
-    </row>
-    <row r="27" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>52</v>
-      </c>
+    <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>